<commit_message>
add new file and delete table of old file
</commit_message>
<xml_diff>
--- a/Чек-лист для Литеры-7 (в каскаде 5.4.6.210).xlsx
+++ b/Чек-лист для Литеры-7 (в каскаде 5.4.6.210).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\p.larionov\Desktop\Документы\Тестовая документация\Литера 7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14209FFA-C282-4934-BD4C-17F2826EC704}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF5896E6-68EF-4B8E-A572-1753DAF3D978}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="7980" xr2:uid="{16B44443-8837-47D1-A5DC-036A1A093821}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="209">
   <si>
     <t>Название тест-кейса</t>
   </si>
@@ -685,134 +685,6 @@
   </si>
   <si>
     <t>Поиск по КС по правилу "К-Р СОСТАВНЫЕ" с перестановкой компонент</t>
-  </si>
-  <si>
-    <t>Индекс у пассажира П
-Пассажир брался из БД pakdb таблица OU_List</t>
-  </si>
-  <si>
-    <t>Проверка поиска по контрольнуму списку (КС) в "Каскад" по правилу с индексом "П", без ошибок в ФИО</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу с индексом "Д", без ошибок в ФИО</t>
-  </si>
-  <si>
-    <t>Индекс у пассажира Д
-Пассажир брался из БД pakdb таблица OU_List</t>
-  </si>
-  <si>
-    <t>Поиск по контрольнуму списку по правилу с индексом "П"</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу  с индексом "Д"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Поиск по КС по правилу с индексом "К" </t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу с идексом "К", без ошибок в ФИО</t>
-  </si>
-  <si>
-    <t>Индекс у пассажира К
-Пассажир брался из БД pakdb таблица OU_List</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Поиск по КС по правилу с индексом "Р" </t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу с индексом "Р", без ошибок в ФИО</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Поиск по КС по правилу с индексом "З" </t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу с индексом "З", без ошибок в ФИО</t>
-  </si>
-  <si>
-    <t>Индекс у пассажира З
-Пассажир брался из БД pakdb таблица OU_List</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Поиск по КС по правилу с индексом "Н" </t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу с индексом "Н", без ошибок в ФИО</t>
-  </si>
-  <si>
-    <t>Индекс у пассажира Н
-Пассажир брался из БД pakdb таблица OU_List</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу с индексом "Т"</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу с индекссом "Т", без ошибок в ФИО</t>
-  </si>
-  <si>
-    <t>Индекс у пассажира Т
-Пассажир брался из БД pakdb таблица OU_List</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Поиск по КС по правилу с индексом "Ф" </t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу с ииндексом "С"</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу с индексом "Ф", без ошибок в ФИО</t>
-  </si>
-  <si>
-    <t>Индекс у пассажира Ф
-Пассажир брался из БД pakdb таблица OU_List</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу с индексом "С", без ошибок в ФИО</t>
-  </si>
-  <si>
-    <t>Индекс у пассажира С
-Пассажир брался из БД pakdb таблица OU_List</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу с инщдексом "В"</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу с индексом "В", без ошибок в ФИО</t>
-  </si>
-  <si>
-    <t>Индекс у пассажира В
-Пассажир брался из БД pakdb таблица OU_List</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Дублирующие тесты, но тут должны быть разные правила
-Надо подумать как их описать</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу с индексом "П" с одной ошибкой в ФИО</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу с индексом "П" с двумя ошибками в ФИО</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу с индексом "П" с тремя ошибками в ФИО</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу с индексом "П" с одной ошибкой в ФИО</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу с индексом "П" с двумя ошибками в ФИО</t>
-  </si>
-  <si>
-    <t>Индекс у пассажира П 
-Пассажир брался из БД pakdb таблица OU_List</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу с индексом "П" с тремя ошибками в ФИО</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "Д"с одна ошибкой в ФИО</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "Д"с двумя ошибками в ФИО</t>
   </si>
 </sst>
 </file>
@@ -859,24 +731,12 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -906,7 +766,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -918,27 +778,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1255,10 +1094,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AB8CD5F-9619-49F5-B4B2-D9FCF71EB8B8}">
-  <dimension ref="A1:J90"/>
+  <dimension ref="A1:D90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1275,7 +1114,7 @@
     <col min="14" max="14" width="35" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1288,34 +1127,16 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="F2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:10" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:4" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -1328,20 +1149,8 @@
       <c r="D3" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:4" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>23</v>
       </c>
@@ -1354,20 +1163,8 @@
       <c r="D4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:4" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>24</v>
       </c>
@@ -1380,20 +1177,8 @@
       <c r="D5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:4" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>25</v>
       </c>
@@ -1406,20 +1191,8 @@
       <c r="D6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:4" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>26</v>
       </c>
@@ -1432,20 +1205,8 @@
       <c r="D7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:4" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>27</v>
       </c>
@@ -1458,20 +1219,8 @@
       <c r="D8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:4" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
@@ -1484,20 +1233,8 @@
       <c r="D9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:4" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>29</v>
       </c>
@@ -1510,20 +1247,8 @@
       <c r="D10" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:4" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>39</v>
       </c>
@@ -1536,20 +1261,8 @@
       <c r="D11" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F11" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:4" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>42</v>
       </c>
@@ -1562,20 +1275,8 @@
       <c r="D12" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F12" s="9" t="s">
-        <v>235</v>
-      </c>
-      <c r="G12" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="H12" s="11" t="s">
-        <v>236</v>
-      </c>
-      <c r="I12" s="11" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:4" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>45</v>
       </c>
@@ -1588,23 +1289,8 @@
       <c r="D13" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="F13" s="5" t="s">
-        <v>235</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>236</v>
-      </c>
-      <c r="I13" s="7" t="s">
-        <v>237</v>
-      </c>
-      <c r="J13" s="8" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:4" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>48</v>
       </c>
@@ -1617,20 +1303,8 @@
       <c r="D14" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F14" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="H14" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="I14" s="7" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:4" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>51</v>
       </c>
@@ -1643,20 +1317,8 @@
       <c r="D15" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F15" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="H15" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="I15" s="7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="69" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:4" ht="69" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>9</v>
       </c>
@@ -1669,20 +1331,8 @@
       <c r="D16" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F16" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="I16" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:4" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>55</v>
       </c>
@@ -1695,20 +1345,8 @@
       <c r="D17" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F17" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="H17" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="I17" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:4" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>56</v>
       </c>
@@ -1721,20 +1359,8 @@
       <c r="D18" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F18" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="H18" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="I18" s="7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:4" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>59</v>
       </c>
@@ -1747,20 +1373,8 @@
       <c r="D19" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="F19" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="H19" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="I19" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>14</v>
       </c>
@@ -1773,20 +1387,8 @@
       <c r="D20" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F20" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="H20" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="I20" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:4" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>62</v>
       </c>
@@ -1799,20 +1401,8 @@
       <c r="D21" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F21" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="G21" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="H21" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="I21" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:4" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>65</v>
       </c>
@@ -1825,20 +1415,8 @@
       <c r="D22" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="F22" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="G22" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="H22" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="I22" s="7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:4" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>68</v>
       </c>
@@ -1851,20 +1429,8 @@
       <c r="D23" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="F23" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="G23" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="H23" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="I23" s="7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:4" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>13</v>
       </c>
@@ -1877,20 +1443,8 @@
       <c r="D24" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="F24" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G24" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="H24" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="I24" s="7" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:4" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>73</v>
       </c>
@@ -1903,20 +1457,8 @@
       <c r="D25" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="F25" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="G25" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="H25" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="I25" s="7" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:4" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>76</v>
       </c>
@@ -1929,20 +1471,8 @@
       <c r="D26" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="F26" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="G26" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="H26" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="I26" s="7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:4" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>153</v>
       </c>
@@ -1955,20 +1485,8 @@
       <c r="D27" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="F27" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="G27" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="H27" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="I27" s="7" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:4" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>79</v>
       </c>
@@ -1981,20 +1499,8 @@
       <c r="D28" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="F28" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="G28" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="H28" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="I28" s="7" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:4" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>82</v>
       </c>
@@ -2007,20 +1513,8 @@
       <c r="D29" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="F29" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="G29" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="H29" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="I29" s="7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:4" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>11</v>
       </c>
@@ -2033,20 +1527,8 @@
       <c r="D30" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="F30" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G30" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="H30" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="I30" s="7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:4" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>87</v>
       </c>
@@ -2059,20 +1541,8 @@
       <c r="D31" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="F31" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="G31" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="H31" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="I31" s="7" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:4" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>90</v>
       </c>
@@ -2085,20 +1555,8 @@
       <c r="D32" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="F32" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="G32" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="H32" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="I32" s="7" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:4" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>155</v>
       </c>
@@ -2111,34 +1569,16 @@
       <c r="D33" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="F33" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="G33" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="H33" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="I33" s="7" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>93</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
-      <c r="F34" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
-    </row>
-    <row r="35" spans="1:9" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:4" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>16</v>
       </c>
@@ -2151,20 +1591,8 @@
       <c r="D35" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F35" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="G35" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H35" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="I35" s="2" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:4" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>94</v>
       </c>
@@ -2177,20 +1605,8 @@
       <c r="D36" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F36" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="G36" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H36" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="I36" s="2" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:4" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>95</v>
       </c>
@@ -2203,20 +1619,8 @@
       <c r="D37" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F37" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="G37" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H37" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="I37" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:4" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>96</v>
       </c>
@@ -2229,20 +1633,8 @@
       <c r="D38" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F38" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="G38" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H38" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="87" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:4" ht="87" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>99</v>
       </c>
@@ -2255,20 +1647,8 @@
       <c r="D39" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F39" s="3" t="s">
-        <v>247</v>
-      </c>
-      <c r="G39" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H39" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="I39" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>107</v>
       </c>
@@ -2281,20 +1661,8 @@
       <c r="D40" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F40" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="G40" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H40" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="I40" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:4" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>19</v>
       </c>
@@ -2307,20 +1675,8 @@
       <c r="D41" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F41" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G41" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H41" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="I41" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:4" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>22</v>
       </c>
@@ -2333,20 +1689,8 @@
       <c r="D42" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F42" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G42" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H42" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="I42" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:4" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>108</v>
       </c>
@@ -2359,20 +1703,8 @@
       <c r="D43" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F43" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="G43" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H43" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="I43" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:4" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>110</v>
       </c>
@@ -2385,20 +1717,8 @@
       <c r="D44" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F44" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="G44" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H44" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="I44" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:4" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>150</v>
       </c>
@@ -2411,20 +1731,8 @@
       <c r="D45" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="F45" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="G45" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H45" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="I45" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:4" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>114</v>
       </c>
@@ -2437,20 +1745,8 @@
       <c r="D46" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="F46" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="G46" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H46" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="I46" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:4" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>115</v>
       </c>
@@ -2463,20 +1759,8 @@
       <c r="D47" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="F47" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="G47" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H47" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="I47" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:4" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>118</v>
       </c>
@@ -2489,20 +1773,8 @@
       <c r="D48" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="F48" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="G48" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H48" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="I48" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>121</v>
       </c>
@@ -2515,20 +1787,8 @@
       <c r="D49" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="F49" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="G49" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H49" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="I49" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:4" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>123</v>
       </c>
@@ -2541,20 +1801,8 @@
       <c r="D50" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="F50" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="G50" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H50" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="I50" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:4" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>124</v>
       </c>
@@ -2567,20 +1815,8 @@
       <c r="D51" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F51" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="G51" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H51" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="I51" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:4" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>127</v>
       </c>
@@ -2593,20 +1829,8 @@
       <c r="D52" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F52" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="G52" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H52" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="I52" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:4" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>128</v>
       </c>
@@ -2619,20 +1843,8 @@
       <c r="D53" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F53" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="G53" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H53" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="I53" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:4" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>131</v>
       </c>
@@ -2645,20 +1857,8 @@
       <c r="D54" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="F54" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="G54" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H54" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="I54" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:4" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>132</v>
       </c>
@@ -2671,20 +1871,8 @@
       <c r="D55" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F55" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="G55" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H55" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="I55" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:4" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>135</v>
       </c>
@@ -2697,20 +1885,8 @@
       <c r="D56" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F56" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="G56" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H56" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="I56" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:4" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>137</v>
       </c>
@@ -2723,20 +1899,8 @@
       <c r="D57" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="F57" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="G57" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H57" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="I57" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:4" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>139</v>
       </c>
@@ -2749,20 +1913,8 @@
       <c r="D58" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="F58" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="G58" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H58" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="I58" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" ht="96" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:4" ht="96" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>141</v>
       </c>
@@ -2775,20 +1927,8 @@
       <c r="D59" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F59" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="G59" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H59" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="I59" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:4" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>142</v>
       </c>
@@ -2801,20 +1941,8 @@
       <c r="D60" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="F60" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="G60" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H60" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="I60" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" ht="87" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:4" ht="87" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>145</v>
       </c>
@@ -2827,20 +1955,8 @@
       <c r="D61" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="F61" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="G61" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H61" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="I61" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>147</v>
       </c>
@@ -2853,20 +1969,8 @@
       <c r="D62" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F62" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="G62" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H62" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="I62" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:4" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>111</v>
       </c>
@@ -2879,34 +1983,16 @@
       <c r="D63" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="F63" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="G63" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H63" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="I63" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:4" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>158</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
-      <c r="F64" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="G64" s="2"/>
-      <c r="H64" s="2"/>
-      <c r="I64" s="2"/>
-    </row>
-    <row r="65" spans="1:9" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:4" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>208</v>
       </c>
@@ -2919,20 +2005,8 @@
       <c r="D65" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F65" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="G65" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H65" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="I65" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="1:4" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>206</v>
       </c>
@@ -2945,20 +2019,8 @@
       <c r="D66" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F66" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="G66" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H66" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="I66" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="1:4" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>204</v>
       </c>
@@ -2971,20 +2033,8 @@
       <c r="D67" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="F67" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="G67" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H67" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="I67" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" ht="102" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="1:4" ht="102" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>202</v>
       </c>
@@ -2997,20 +2047,8 @@
       <c r="D68" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F68" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="G68" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H68" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="I68" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="1:4" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>200</v>
       </c>
@@ -3023,20 +2061,8 @@
       <c r="D69" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F69" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="G69" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H69" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="I69" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="1:4" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>198</v>
       </c>
@@ -3049,34 +2075,16 @@
       <c r="D70" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="F70" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="G70" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H70" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="I70" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="71" spans="1:4" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>159</v>
       </c>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
-      <c r="F71" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="G71" s="2"/>
-      <c r="H71" s="2"/>
-      <c r="I71" s="2"/>
-    </row>
-    <row r="72" spans="1:9" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="72" spans="1:4" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>196</v>
       </c>
@@ -3089,20 +2097,8 @@
       <c r="D72" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="F72" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="G72" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H72" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="I72" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="73" spans="1:4" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>194</v>
       </c>
@@ -3115,20 +2111,8 @@
       <c r="D73" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="F73" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="G73" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H73" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="I73" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="74" spans="1:4" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>192</v>
       </c>
@@ -3141,20 +2125,8 @@
       <c r="D74" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F74" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="G74" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H74" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="I74" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="75" spans="1:4" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>190</v>
       </c>
@@ -3167,20 +2139,8 @@
       <c r="D75" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F75" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="G75" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H75" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="I75" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="76" spans="1:4" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>188</v>
       </c>
@@ -3193,20 +2153,8 @@
       <c r="D76" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F76" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="G76" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H76" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="I76" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="77" spans="1:4" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>186</v>
       </c>
@@ -3219,20 +2167,8 @@
       <c r="D77" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F77" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="G77" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H77" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="I77" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="1:4" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>184</v>
       </c>
@@ -3245,20 +2181,8 @@
       <c r="D78" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="F78" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="G78" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H78" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="I78" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" ht="99" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="79" spans="1:4" ht="99" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>181</v>
       </c>
@@ -3271,34 +2195,16 @@
       <c r="D79" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F79" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="G79" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H79" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="I79" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="80" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>182</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
       <c r="D80" s="2"/>
-      <c r="F80" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="G80" s="2"/>
-      <c r="H80" s="2"/>
-      <c r="I80" s="2"/>
-    </row>
-    <row r="81" spans="1:9" ht="96" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="81" spans="1:4" ht="96" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>179</v>
       </c>
@@ -3311,20 +2217,8 @@
       <c r="D81" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F81" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="G81" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H81" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="I81" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="82" spans="1:4" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>177</v>
       </c>
@@ -3337,20 +2231,8 @@
       <c r="D82" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F82" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="G82" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H82" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="I82" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="83" spans="1:4" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>175</v>
       </c>
@@ -3363,20 +2245,8 @@
       <c r="D83" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F83" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="G83" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H83" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="I83" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="84" spans="1:4" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
         <v>173</v>
       </c>
@@ -3389,20 +2259,8 @@
       <c r="D84" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F84" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="G84" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H84" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="I84" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="85" spans="1:4" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
         <v>171</v>
       </c>
@@ -3415,20 +2273,8 @@
       <c r="D85" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F85" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="G85" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H85" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="I85" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="86" spans="1:4" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
         <v>169</v>
       </c>
@@ -3441,20 +2287,8 @@
       <c r="D86" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F86" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="G86" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H86" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="I86" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9" ht="267.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="87" spans="1:4" ht="63" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
         <v>167</v>
       </c>
@@ -3467,20 +2301,8 @@
       <c r="D87" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="F87" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="G87" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H87" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="I87" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9" ht="267.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="88" spans="1:4" ht="63" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
         <v>165</v>
       </c>
@@ -3493,20 +2315,8 @@
       <c r="D88" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="F88" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="G88" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H88" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="I88" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="89" spans="1:9" ht="283.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="89" spans="1:4" ht="63" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
         <v>163</v>
       </c>
@@ -3519,20 +2329,8 @@
       <c r="D89" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F89" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="G89" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H89" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="I89" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9" ht="283.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="90" spans="1:4" ht="63" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
         <v>160</v>
       </c>
@@ -3543,18 +2341,6 @@
         <v>161</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F90" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="G90" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H90" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="I90" s="2" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>